<commit_message>
up sms added with issues
</commit_message>
<xml_diff>
--- a/Echo/Router ip list with 37 SMS numbers.xlsx
+++ b/Echo/Router ip list with 37 SMS numbers.xlsx
@@ -17,14 +17,14 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$105</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="350">
   <si>
     <t>Moghbazar</t>
   </si>
@@ -1052,10 +1052,28 @@
     <t>SMSENABLED</t>
   </si>
   <si>
-    <t>123.49.2.80</t>
-  </si>
-  <si>
-    <t>Me</t>
+    <t>192.168.0.206</t>
+  </si>
+  <si>
+    <t>sbn2</t>
+  </si>
+  <si>
+    <t>sbn3</t>
+  </si>
+  <si>
+    <t>5th floor</t>
+  </si>
+  <si>
+    <t>5th floor-2</t>
+  </si>
+  <si>
+    <t>192.168.1.101</t>
+  </si>
+  <si>
+    <t>123.49.2.82</t>
+  </si>
+  <si>
+    <t>Central billing</t>
   </si>
 </sst>
 </file>
@@ -1630,11 +1648,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K101"/>
+  <dimension ref="A1:K105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1663,795 +1681,783 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:11" s="21" customFormat="1">
+      <c r="A2" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>346</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="21" customFormat="1">
+      <c r="A3" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>345</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="21" customFormat="1">
+      <c r="A4" s="22" t="s">
         <v>342</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B4" s="23" t="s">
         <v>343</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D2" s="12" t="s">
+      <c r="C4" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>343</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>259</v>
+    </row>
+    <row r="5" spans="1:11" s="21" customFormat="1">
+      <c r="A5" s="22" t="s">
+        <v>342</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>344</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="K5" s="2"/>
+      <c r="D5" s="23" t="s">
+        <v>344</v>
+      </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>244</v>
+        <v>348</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>349</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="K6" s="1"/>
+      <c r="D6" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="12" t="s">
-        <v>296</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>297</v>
+        <v>107</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>236</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="K7" s="1"/>
+      <c r="D7" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="12" t="s">
-        <v>140</v>
+        <v>184</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>252</v>
+        <v>274</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>134</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>251</v>
+        <v>165</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D9" s="33" t="s">
-        <v>133</v>
-      </c>
+      <c r="D9" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>248</v>
+        <v>122</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>244</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D10" s="33" t="s">
-        <v>120</v>
-      </c>
+      <c r="D10" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>245</v>
+        <v>296</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>297</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D11" s="33" t="s">
-        <v>117</v>
-      </c>
+      <c r="D11" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="B12" s="31" t="s">
-        <v>247</v>
+        <v>140</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>252</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D12" s="12" t="s">
-        <v>119</v>
+      <c r="D12" s="11" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="12" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>270</v>
+        <v>127</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>248</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>158</v>
+      <c r="D14" s="33" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>269</v>
+        <v>123</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>245</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>157</v>
+      <c r="D15" s="33" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="12" t="s">
-        <v>174</v>
+        <v>125</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D16" s="33" t="s">
-        <v>156</v>
+      <c r="D16" s="12" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>235</v>
+        <v>130</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>249</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D17" s="12" t="s">
-        <v>94</v>
+      <c r="D17" s="33" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>242</v>
+      <c r="A18" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>270</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D18" s="20" t="s">
-        <v>100</v>
+      <c r="D18" s="11" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>238</v>
+        <v>175</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>269</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>96</v>
+      <c r="D19" s="11" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>231</v>
+        <v>174</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>268</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D20" s="10" t="s">
-        <v>292</v>
+      <c r="D20" s="33" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="12" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="B22" s="31" t="s">
-        <v>233</v>
+      <c r="A22" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>242</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D22" s="33" t="s">
-        <v>92</v>
+      <c r="D22" s="20" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>241</v>
+      <c r="A23" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>238</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D23" s="20" t="s">
-        <v>99</v>
+      <c r="D23" s="12" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="12" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D24" s="12" t="s">
-        <v>93</v>
+      <c r="D24" s="10" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="12" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>237</v>
+        <v>104</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>233</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D26" s="12" t="s">
-        <v>288</v>
+      <c r="D26" s="33" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="12" t="s">
-        <v>183</v>
+      <c r="A27" s="20" t="s">
+        <v>112</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>273</v>
+        <v>241</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>179</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>190</v>
+      <c r="A28" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>234</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D28" s="20" t="s">
-        <v>10</v>
+      <c r="D28" s="12" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>243</v>
+      <c r="A29" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>239</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D29" s="10" t="s">
-        <v>116</v>
+      <c r="D29" s="12" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="12" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>275</v>
+        <v>237</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B35" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="C31" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D31" s="20" t="s">
+      <c r="C35" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D35" s="20" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="12" t="s">
+    <row r="36" spans="1:4">
+      <c r="A36" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B36" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="C32" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D32" s="12" t="s">
+      <c r="C36" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D36" s="12" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="10" t="s">
+    <row r="37" spans="1:4">
+      <c r="A37" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="C33" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D33" s="10" t="s">
+      <c r="C37" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D37" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="10" t="s">
+    <row r="38" spans="1:4">
+      <c r="A38" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C34" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D34" s="10" t="s">
+      <c r="C38" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D38" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="10" t="s">
+    <row r="39" spans="1:4">
+      <c r="A39" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="C35" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D35" s="10" t="s">
+      <c r="C39" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D39" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="10" t="s">
+    <row r="40" spans="1:4">
+      <c r="A40" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C36" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D36" s="10" t="s">
+      <c r="C40" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D40" s="10" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D37" s="20" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>265</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D39" s="20" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>253</v>
+        <v>182</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>272</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D41" s="13" t="s">
-        <v>142</v>
+      <c r="D41" s="20" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>254</v>
+        <v>171</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>265</v>
       </c>
       <c r="C42" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D42" s="13" t="s">
-        <v>185</v>
+      <c r="D42" s="20" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B47" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="C43" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D43" s="13" t="s">
+      <c r="C47" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D47" s="13" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="B45" s="30" t="s">
-        <v>224</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D45" s="28" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>267</v>
+        <v>168</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>262</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D48" s="9" t="s">
-        <v>155</v>
+      <c r="D48" s="13" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>258</v>
+      <c r="A49" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B49" s="30" t="s">
+        <v>224</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D49" s="13" t="s">
-        <v>146</v>
+      <c r="D49" s="28" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="9" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C50" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D54" s="13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B55" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="C51" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D51" s="13" t="s">
+      <c r="C55" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D55" s="13" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="29" t="s">
+    <row r="56" spans="1:6">
+      <c r="A56" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B56" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="C52" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D52" s="13" t="s">
+      <c r="C56" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D56" s="13" t="s">
         <v>9</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F53" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F54" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="B55" s="30" t="s">
-        <v>209</v>
-      </c>
-      <c r="C55" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D55" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B56" s="30" t="s">
-        <v>197</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>26</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>0</v>
@@ -2459,16 +2465,16 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>188</v>
+        <v>14</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>191</v>
       </c>
       <c r="C57" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D57" s="12" t="s">
-        <v>7</v>
+      <c r="D57" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>0</v>
@@ -2476,16 +2482,16 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>204</v>
+        <v>18</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>193</v>
       </c>
       <c r="C58" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D58" s="10" t="s">
-        <v>40</v>
+      <c r="D58" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>0</v>
@@ -2493,16 +2499,16 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="28" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="B59" s="30" t="s">
-        <v>186</v>
+        <v>209</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D59" s="28" t="s">
-        <v>285</v>
+        <v>51</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>0</v>
@@ -2510,16 +2516,16 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="28" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B60" s="30" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="C60" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D60" s="28" t="s">
-        <v>4</v>
+      <c r="D60" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="F60" s="7" t="s">
         <v>0</v>
@@ -2527,16 +2533,16 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B61" s="30" t="s">
-        <v>198</v>
+        <v>8</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>188</v>
       </c>
       <c r="C61" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D61" s="28" t="s">
-        <v>27</v>
+      <c r="D61" s="12" t="s">
+        <v>7</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>0</v>
@@ -2544,31 +2550,33 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="28" t="s">
-        <v>298</v>
-      </c>
-      <c r="B62" s="30" t="s">
-        <v>299</v>
+        <v>39</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>204</v>
       </c>
       <c r="C62" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D62" s="28" t="s">
-        <v>300</v>
-      </c>
-      <c r="F62" s="7"/>
+      <c r="D62" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>192</v>
+        <v>6</v>
+      </c>
+      <c r="B63" s="30" t="s">
+        <v>186</v>
       </c>
       <c r="C63" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D63" s="9" t="s">
-        <v>15</v>
+      <c r="D63" s="28" t="s">
+        <v>285</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>0</v>
@@ -2576,541 +2584,607 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>199</v>
+        <v>5</v>
+      </c>
+      <c r="B64" s="30" t="s">
+        <v>187</v>
       </c>
       <c r="C64" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D64" s="9" t="s">
-        <v>29</v>
+      <c r="D64" s="28" t="s">
+        <v>4</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:6">
       <c r="A65" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B65" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D65" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B66" s="30" t="s">
+        <v>299</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D66" s="28" t="s">
+        <v>300</v>
+      </c>
+      <c r="F66" s="7"/>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="B65" s="30" t="s">
+      <c r="B69" s="30" t="s">
         <v>215</v>
       </c>
-      <c r="C65" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D65" s="28" t="s">
+      <c r="C69" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D69" s="28" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="28" t="s">
+    <row r="70" spans="1:6">
+      <c r="A70" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="B66" s="30" t="s">
+      <c r="B70" s="30" t="s">
         <v>205</v>
       </c>
-      <c r="C66" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D66" s="28" t="s">
+      <c r="C70" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D70" s="28" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="28" t="s">
+    <row r="71" spans="1:6">
+      <c r="A71" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B67" s="30" t="s">
+      <c r="B71" s="30" t="s">
         <v>206</v>
       </c>
-      <c r="C67" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D67" s="28" t="s">
+      <c r="C71" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D71" s="28" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="28" t="s">
+    <row r="72" spans="1:6">
+      <c r="A72" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B68" s="30" t="s">
+      <c r="B72" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="C68" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D68" s="28" t="s">
+      <c r="C72" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D72" s="28" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="9" t="s">
+    <row r="73" spans="1:6">
+      <c r="A73" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B73" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="C69" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D69" s="9" t="s">
+      <c r="C73" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D73" s="9" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="13" t="s">
+    <row r="74" spans="1:6">
+      <c r="A74" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="B70" s="8" t="s">
+      <c r="B74" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="C70" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D70" s="13" t="s">
+      <c r="C74" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D74" s="13" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="13" t="s">
+    <row r="75" spans="1:6">
+      <c r="A75" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="B71" s="8" t="s">
+      <c r="B75" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="C71" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D71" s="13" t="s">
+      <c r="C75" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D75" s="13" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="9" t="s">
+    <row r="76" spans="1:6">
+      <c r="A76" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="B72" s="7" t="s">
+      <c r="B76" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="C72" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D72" s="9" t="s">
+      <c r="C76" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D76" s="9" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="28" t="s">
+    <row r="77" spans="1:6">
+      <c r="A77" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="B73" s="30" t="s">
+      <c r="B77" s="30" t="s">
         <v>222</v>
       </c>
-      <c r="C73" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D73" s="28" t="s">
+      <c r="C77" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D77" s="28" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="28" t="s">
+    <row r="78" spans="1:6">
+      <c r="A78" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="B74" s="30" t="s">
+      <c r="B78" s="30" t="s">
         <v>221</v>
       </c>
-      <c r="C74" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D74" s="28" t="s">
+      <c r="C78" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D78" s="28" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="16" t="s">
+    <row r="79" spans="1:6">
+      <c r="A79" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B75" s="32" t="s">
+      <c r="B79" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="C75" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D75" s="35" t="s">
+      <c r="C79" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D79" s="35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="28" t="s">
+    <row r="80" spans="1:6">
+      <c r="A80" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="B76" s="30" t="s">
+      <c r="B80" s="30" t="s">
         <v>218</v>
       </c>
-      <c r="C76" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D76" s="28" t="s">
+      <c r="C80" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D80" s="28" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="B77" s="30" t="s">
-        <v>225</v>
-      </c>
-      <c r="C77" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D77" s="28" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="B78" s="30" t="s">
-        <v>223</v>
-      </c>
-      <c r="C78" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D78" s="28" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="C79" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D79" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="C80" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D80" s="9" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="28" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="B81" s="30" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="C81" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D81" s="28" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>228</v>
+        <v>77</v>
+      </c>
+      <c r="B82" s="30" t="s">
+        <v>223</v>
       </c>
       <c r="C82" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D82" s="9" t="s">
-        <v>86</v>
+      <c r="D82" s="28" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="B83" s="30" t="s">
-        <v>216</v>
+        <v>88</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>227</v>
       </c>
       <c r="C83" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D83" s="37" t="s">
-        <v>64</v>
+      <c r="D83" s="9" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="B84" s="30" t="s">
-        <v>217</v>
+        <v>90</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>229</v>
       </c>
       <c r="C84" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D84" s="28" t="s">
-        <v>70</v>
+      <c r="D84" s="9" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B85" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D85" s="28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C86" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D86" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B87" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="C87" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D87" s="37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B88" s="30" t="s">
+        <v>217</v>
+      </c>
+      <c r="C88" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D88" s="28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="28" t="s">
         <v>301</v>
       </c>
-      <c r="B85" s="30" t="s">
+      <c r="B89" s="30" t="s">
         <v>302</v>
       </c>
-      <c r="C85" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D85" s="37" t="s">
+      <c r="C89" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D89" s="37" t="s">
         <v>303</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
-      <c r="A86" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="C86" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D86" s="9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4">
-      <c r="A87" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="C87" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D87" s="9" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
-      <c r="A88" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="B88" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="C88" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D88" s="19" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="B89" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="C89" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D89" s="9" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C90" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="C91" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D91" s="9" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="C92" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D92" s="19" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C93" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D93" s="9" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="B90" s="7" t="s">
+      <c r="B94" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="C90" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D90" s="9" t="s">
+      <c r="C94" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D94" s="9" t="s">
         <v>282</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4">
-      <c r="A91" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B91" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="C91" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D91" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
-      <c r="A92" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B92" s="30" t="s">
-        <v>202</v>
-      </c>
-      <c r="C92" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D92" s="28" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
-      <c r="A93" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="B93" s="30" t="s">
-        <v>208</v>
-      </c>
-      <c r="C93" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D93" s="28" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4">
-      <c r="A94" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="B94" s="30" t="s">
-        <v>213</v>
-      </c>
-      <c r="C94" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D94" s="36" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="B95" s="30" t="s">
-        <v>214</v>
+        <v>34</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>203</v>
       </c>
       <c r="C95" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D95" s="28" t="s">
-        <v>61</v>
+      <c r="D95" s="9" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="28" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B96" s="30" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C96" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D96" s="34" t="s">
-        <v>53</v>
+      <c r="D96" s="28" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="28" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B97" s="30" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C97" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D97" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="28" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B98" s="30" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C98" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D98" s="10" t="s">
-        <v>55</v>
+      <c r="D98" s="36" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="B99" s="7" t="s">
-        <v>279</v>
+      <c r="A99" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B99" s="30" t="s">
+        <v>214</v>
       </c>
       <c r="C99" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D99" s="9" t="s">
-        <v>284</v>
+      <c r="D99" s="28" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="B100" s="7" t="s">
-        <v>200</v>
+        <v>54</v>
+      </c>
+      <c r="B100" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C100" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D100" s="18" t="s">
-        <v>30</v>
+      <c r="D100" s="34" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B101" s="30" t="s">
+        <v>210</v>
+      </c>
+      <c r="C101" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D101" s="28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B102" s="30" t="s">
+        <v>212</v>
+      </c>
+      <c r="C102" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D102" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="C103" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D103" s="9" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C104" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D104" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B101" s="7" t="s">
+      <c r="B105" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="C101" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D101" s="9" t="s">
+      <c r="C105" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D105" s="9" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D101">
+  <autoFilter ref="A1:D105">
     <sortState ref="A2:E102">
       <sortCondition ref="D2:D102"/>
     </sortState>

</xml_diff>

<commit_message>
status change sms completed
</commit_message>
<xml_diff>
--- a/Echo/Router ip list with 37 SMS numbers.xlsx
+++ b/Echo/Router ip list with 37 SMS numbers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Echo\Echo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Echo\Echo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1653,9 +1653,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3212,7 +3212,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
solved excel button issue & fluctuation issue
</commit_message>
<xml_diff>
--- a/Echo/Router ip list with 37 SMS numbers.xlsx
+++ b/Echo/Router ip list with 37 SMS numbers.xlsx
@@ -17,14 +17,14 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$105</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$103</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="349">
   <si>
     <t>Moghbazar</t>
   </si>
@@ -1061,12 +1061,6 @@
     <t>192.168.1.101</t>
   </si>
   <si>
-    <t>123.49.2.82</t>
-  </si>
-  <si>
-    <t>Central billing</t>
-  </si>
-  <si>
     <t>5th floor Phone</t>
   </si>
   <si>
@@ -1077,15 +1071,6 @@
   </si>
   <si>
     <t>192.168.0.207</t>
-  </si>
-  <si>
-    <t>192.168.0.208</t>
-  </si>
-  <si>
-    <t>5th floor PC 2</t>
-  </si>
-  <si>
-    <t>PC 2</t>
   </si>
 </sst>
 </file>
@@ -1660,11 +1645,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K105"/>
+  <dimension ref="A1:K103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1695,781 +1680,784 @@
     </row>
     <row r="2" spans="1:11" s="26" customFormat="1">
       <c r="A2" s="12" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>341</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="26" customFormat="1">
       <c r="A3" s="12" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>341</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>349</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="26" customFormat="1">
       <c r="A4" s="12" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>341</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="26" customFormat="1">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="12" t="s">
-        <v>342</v>
+        <v>107</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>343</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>343</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="12" t="s">
-        <v>345</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>346</v>
+        <v>184</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>274</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="D6" s="11" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>236</v>
+        <v>165</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="D7" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="12" t="s">
-        <v>184</v>
+        <v>122</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>274</v>
+        <v>244</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>180</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="12" t="s">
-        <v>165</v>
+        <v>296</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>259</v>
+        <v>297</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="K9" s="2"/>
+        <v>131</v>
+      </c>
+      <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="12" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="K10" s="1"/>
+        <v>134</v>
+      </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="12" t="s">
-        <v>296</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>297</v>
+        <v>139</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>251</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="K11" s="1"/>
+      <c r="D11" s="33" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>252</v>
+        <v>127</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>248</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>134</v>
+      <c r="D12" s="33" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="12" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D14" s="33" t="s">
-        <v>120</v>
+      <c r="D14" s="12" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="12" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="B16" s="31" t="s">
-        <v>247</v>
+        <v>176</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>270</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D16" s="12" t="s">
-        <v>119</v>
+      <c r="D16" s="11" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="B17" s="31" t="s">
-        <v>249</v>
+        <v>175</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>269</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D17" s="33" t="s">
-        <v>121</v>
+      <c r="D17" s="11" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>270</v>
+        <v>174</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>268</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>158</v>
+      <c r="D18" s="33" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>269</v>
+        <v>106</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>235</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>157</v>
+      <c r="D19" s="12" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="B20" s="31" t="s">
-        <v>268</v>
+      <c r="A20" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>242</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D20" s="33" t="s">
-        <v>156</v>
+      <c r="D20" s="20" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="12" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>242</v>
+      <c r="A22" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>231</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D22" s="20" t="s">
-        <v>100</v>
+      <c r="D22" s="10" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="12" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>231</v>
+        <v>104</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>233</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D24" s="10" t="s">
-        <v>292</v>
+      <c r="D24" s="33" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>230</v>
+      <c r="A25" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>241</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D25" s="12" t="s">
-        <v>114</v>
+      <c r="D25" s="20" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="B26" s="31" t="s">
-        <v>233</v>
+        <v>105</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>234</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D26" s="33" t="s">
-        <v>92</v>
+      <c r="D26" s="12" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>241</v>
+      <c r="A27" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>239</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D27" s="20" t="s">
-        <v>99</v>
+      <c r="D27" s="12" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="12" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>93</v>
+        <v>288</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>239</v>
+        <v>183</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>273</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D29" s="12" t="s">
-        <v>97</v>
+      <c r="D29" s="20" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>237</v>
+      <c r="A30" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>190</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D30" s="12" t="s">
-        <v>288</v>
+      <c r="D30" s="20" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>273</v>
+      <c r="A31" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>243</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D31" s="20" t="s">
-        <v>179</v>
+      <c r="D31" s="10" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>190</v>
+      <c r="A32" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>275</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D32" s="20" t="s">
-        <v>10</v>
+      <c r="D32" s="12" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>243</v>
+      <c r="A33" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>255</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D33" s="10" t="s">
-        <v>116</v>
+      <c r="D33" s="20" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="12" t="s">
-        <v>128</v>
+        <v>172</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>280</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>255</v>
+      <c r="A35" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>196</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D35" s="20" t="s">
-        <v>143</v>
+      <c r="D35" s="10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>266</v>
+      <c r="A36" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D36" s="12" t="s">
-        <v>154</v>
+      <c r="D36" s="10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="10" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>194</v>
+        <v>226</v>
       </c>
       <c r="C38" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>195</v>
+      <c r="A39" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>272</v>
       </c>
       <c r="C39" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D39" s="10" t="s">
-        <v>22</v>
+      <c r="D39" s="20" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>226</v>
+      <c r="A40" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>265</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D40" s="10" t="s">
-        <v>84</v>
+      <c r="D40" s="20" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="12" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>178</v>
+        <v>149</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="B42" s="17" t="s">
-        <v>265</v>
+        <v>166</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>260</v>
       </c>
       <c r="C42" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D42" s="20" t="s">
-        <v>153</v>
+      <c r="D42" s="12" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>261</v>
+        <v>159</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>253</v>
       </c>
       <c r="C43" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D43" s="20" t="s">
-        <v>149</v>
+      <c r="D43" s="13" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>260</v>
+        <v>160</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>254</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D44" s="12" t="s">
-        <v>148</v>
+      <c r="D44" s="13" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="12" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C45" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="12" t="s">
-        <v>160</v>
+      <c r="A46" s="9" t="s">
+        <v>168</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="C46" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>185</v>
+        <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>257</v>
+      <c r="A47" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47" s="30" t="s">
+        <v>224</v>
       </c>
       <c r="C47" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D47" s="13" t="s">
-        <v>145</v>
+      <c r="D47" s="28" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="9" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="B49" s="30" t="s">
-        <v>224</v>
+      <c r="A49" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>263</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D49" s="28" t="s">
-        <v>80</v>
+      <c r="D49" s="9" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>256</v>
+        <v>173</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>267</v>
       </c>
       <c r="C50" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D50" s="13" t="s">
-        <v>144</v>
+      <c r="D50" s="9" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>263</v>
+        <v>164</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>258</v>
       </c>
       <c r="C51" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D51" s="9" t="s">
-        <v>151</v>
+      <c r="D51" s="13" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>267</v>
+        <v>170</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>264</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D52" s="9" t="s">
-        <v>155</v>
+      <c r="D52" s="13" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="9" t="s">
-        <v>164</v>
+        <v>181</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>258</v>
+        <v>271</v>
       </c>
       <c r="C53" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>146</v>
+        <v>177</v>
       </c>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="9" t="s">
-        <v>170</v>
+      <c r="A54" s="29" t="s">
+        <v>12</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>264</v>
+        <v>189</v>
       </c>
       <c r="C54" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D54" s="13" t="s">
-        <v>152</v>
+        <v>9</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>271</v>
+      <c r="A55" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>191</v>
       </c>
       <c r="C55" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D55" s="13" t="s">
-        <v>177</v>
+      <c r="D55" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>189</v>
+      <c r="A56" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>193</v>
       </c>
       <c r="C56" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D56" s="13" t="s">
-        <v>9</v>
+      <c r="D56" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>0</v>
@@ -2477,16 +2465,16 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>191</v>
+        <v>52</v>
+      </c>
+      <c r="B57" s="30" t="s">
+        <v>209</v>
       </c>
       <c r="C57" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D57" s="9" t="s">
-        <v>11</v>
+      <c r="D57" s="28" t="s">
+        <v>51</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>0</v>
@@ -2494,16 +2482,16 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>193</v>
+        <v>25</v>
+      </c>
+      <c r="B58" s="30" t="s">
+        <v>197</v>
       </c>
       <c r="C58" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>0</v>
@@ -2511,16 +2499,16 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="B59" s="30" t="s">
-        <v>209</v>
+        <v>8</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>188</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D59" s="28" t="s">
-        <v>51</v>
+      <c r="D59" s="12" t="s">
+        <v>7</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>0</v>
@@ -2528,16 +2516,16 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B60" s="30" t="s">
-        <v>197</v>
+        <v>39</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>204</v>
       </c>
       <c r="C60" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D60" s="9" t="s">
-        <v>26</v>
+      <c r="D60" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="F60" s="7" t="s">
         <v>0</v>
@@ -2545,16 +2533,16 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>188</v>
+        <v>6</v>
+      </c>
+      <c r="B61" s="30" t="s">
+        <v>186</v>
       </c>
       <c r="C61" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D61" s="12" t="s">
-        <v>7</v>
+      <c r="D61" s="28" t="s">
+        <v>285</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>0</v>
@@ -2562,16 +2550,16 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>204</v>
+        <v>5</v>
+      </c>
+      <c r="B62" s="30" t="s">
+        <v>187</v>
       </c>
       <c r="C62" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D62" s="10" t="s">
-        <v>40</v>
+      <c r="D62" s="28" t="s">
+        <v>4</v>
       </c>
       <c r="F62" s="7" t="s">
         <v>0</v>
@@ -2579,16 +2567,16 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="28" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B63" s="30" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="C63" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D63" s="28" t="s">
-        <v>285</v>
+        <v>27</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>0</v>
@@ -2596,33 +2584,31 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="28" t="s">
-        <v>5</v>
+        <v>298</v>
       </c>
       <c r="B64" s="30" t="s">
-        <v>187</v>
+        <v>299</v>
       </c>
       <c r="C64" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D64" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="F64" s="7" t="s">
-        <v>0</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="F64" s="7"/>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B65" s="30" t="s">
-        <v>198</v>
+        <v>16</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>192</v>
       </c>
       <c r="C65" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D65" s="28" t="s">
-        <v>27</v>
+      <c r="D65" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="F65" s="7" t="s">
         <v>0</v>
@@ -2630,573 +2616,541 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="28" t="s">
-        <v>298</v>
-      </c>
-      <c r="B66" s="30" t="s">
-        <v>299</v>
+        <v>32</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="C66" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D66" s="28" t="s">
-        <v>300</v>
-      </c>
-      <c r="F66" s="7"/>
+      <c r="D66" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>192</v>
+        <v>59</v>
+      </c>
+      <c r="B67" s="30" t="s">
+        <v>215</v>
       </c>
       <c r="C67" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D67" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F67" s="7" t="s">
-        <v>0</v>
+      <c r="D67" s="28" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>199</v>
+        <v>41</v>
+      </c>
+      <c r="B68" s="30" t="s">
+        <v>205</v>
       </c>
       <c r="C68" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D68" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F68" s="7" t="s">
-        <v>0</v>
+      <c r="D68" s="28" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="28" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B69" s="30" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C69" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D69" s="28" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="28" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B70" s="30" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C70" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D70" s="28" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="B71" s="30" t="s">
-        <v>206</v>
+      <c r="A71" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>287</v>
       </c>
       <c r="C71" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D71" s="28" t="s">
-        <v>43</v>
+      <c r="D71" s="9" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="B72" s="30" t="s">
-        <v>207</v>
+      <c r="A72" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>232</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D72" s="28" t="s">
-        <v>45</v>
+      <c r="D72" s="13" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>287</v>
+      <c r="A73" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>240</v>
       </c>
       <c r="C73" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D73" s="9" t="s">
-        <v>286</v>
+      <c r="D73" s="13" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:6">
-      <c r="A74" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="B74" s="8" t="s">
-        <v>232</v>
+      <c r="A74" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>250</v>
       </c>
       <c r="C74" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D74" s="13" t="s">
-        <v>91</v>
+      <c r="D74" s="9" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="75" spans="1:6">
-      <c r="A75" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>240</v>
+      <c r="A75" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="B75" s="30" t="s">
+        <v>222</v>
       </c>
       <c r="C75" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D75" s="13" t="s">
-        <v>98</v>
+      <c r="D75" s="28" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="76" spans="1:6">
-      <c r="A76" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>250</v>
+      <c r="A76" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B76" s="30" t="s">
+        <v>221</v>
       </c>
       <c r="C76" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D76" s="9" t="s">
-        <v>132</v>
+      <c r="D76" s="28" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:6">
-      <c r="A77" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="B77" s="30" t="s">
-        <v>222</v>
+      <c r="A77" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B77" s="32" t="s">
+        <v>220</v>
       </c>
       <c r="C77" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D77" s="28" t="s">
-        <v>76</v>
+      <c r="D77" s="35" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="28" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B78" s="30" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C78" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D78" s="28" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="79" spans="1:6">
-      <c r="A79" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B79" s="32" t="s">
-        <v>220</v>
+      <c r="A79" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B79" s="30" t="s">
+        <v>225</v>
       </c>
       <c r="C79" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D79" s="35" t="s">
-        <v>73</v>
+      <c r="D79" s="28" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="28" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B80" s="30" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="C80" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="B81" s="30" t="s">
-        <v>225</v>
+        <v>88</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>227</v>
       </c>
       <c r="C81" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D81" s="28" t="s">
-        <v>83</v>
+      <c r="D81" s="9" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="B82" s="30" t="s">
-        <v>223</v>
+        <v>90</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>229</v>
       </c>
       <c r="C82" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D82" s="28" t="s">
-        <v>79</v>
+      <c r="D82" s="9" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>227</v>
+        <v>67</v>
+      </c>
+      <c r="B83" s="30" t="s">
+        <v>219</v>
       </c>
       <c r="C83" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D83" s="9" t="s">
-        <v>85</v>
+      <c r="D83" s="28" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C84" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="28" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B85" s="30" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C85" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D85" s="28" t="s">
-        <v>72</v>
+      <c r="D85" s="37" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>228</v>
+        <v>65</v>
+      </c>
+      <c r="B86" s="30" t="s">
+        <v>217</v>
       </c>
       <c r="C86" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D86" s="9" t="s">
-        <v>86</v>
+      <c r="D86" s="28" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="28" t="s">
-        <v>63</v>
+        <v>301</v>
       </c>
       <c r="B87" s="30" t="s">
-        <v>216</v>
+        <v>302</v>
       </c>
       <c r="C87" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D87" s="37" t="s">
-        <v>64</v>
+        <v>303</v>
       </c>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="B88" s="30" t="s">
-        <v>217</v>
+      <c r="A88" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>246</v>
       </c>
       <c r="C88" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D88" s="28" t="s">
-        <v>70</v>
+      <c r="D88" s="9" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="28" t="s">
-        <v>301</v>
-      </c>
-      <c r="B89" s="30" t="s">
-        <v>302</v>
+      <c r="A89" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>276</v>
       </c>
       <c r="C89" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D89" s="37" t="s">
-        <v>303</v>
+      <c r="D89" s="9" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="9" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>246</v>
+        <v>278</v>
       </c>
       <c r="C90" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D90" s="9" t="s">
-        <v>118</v>
+      <c r="D90" s="19" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="9" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>276</v>
+        <v>294</v>
       </c>
       <c r="C91" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>281</v>
+        <v>293</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C92" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D92" s="19" t="s">
-        <v>283</v>
+      <c r="D92" s="9" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="93" spans="1:4">
-      <c r="A93" s="9" t="s">
-        <v>135</v>
+      <c r="A93" s="28" t="s">
+        <v>34</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>294</v>
+        <v>203</v>
       </c>
       <c r="C93" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>293</v>
+        <v>31</v>
       </c>
     </row>
     <row r="94" spans="1:4">
-      <c r="A94" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="B94" s="7" t="s">
-        <v>277</v>
+      <c r="A94" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B94" s="30" t="s">
+        <v>202</v>
       </c>
       <c r="C94" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D94" s="9" t="s">
-        <v>282</v>
+      <c r="D94" s="28" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B95" s="7" t="s">
-        <v>203</v>
+        <v>47</v>
+      </c>
+      <c r="B95" s="30" t="s">
+        <v>208</v>
       </c>
       <c r="C95" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D95" s="9" t="s">
-        <v>31</v>
+      <c r="D95" s="28" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="28" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B96" s="30" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="C96" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D96" s="28" t="s">
-        <v>38</v>
+      <c r="D96" s="36" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="28" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B97" s="30" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="C97" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D97" s="28" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="28" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B98" s="30" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C98" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D98" s="36" t="s">
-        <v>58</v>
+      <c r="D98" s="34" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="28" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B99" s="30" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C99" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D99" s="28" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="28" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B100" s="30" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C100" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D100" s="34" t="s">
-        <v>53</v>
+      <c r="D100" s="10" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B101" s="30" t="s">
-        <v>210</v>
+      <c r="A101" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="C101" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D101" s="28" t="s">
-        <v>49</v>
+      <c r="D101" s="9" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="B102" s="30" t="s">
-        <v>212</v>
+        <v>33</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="C102" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D102" s="10" t="s">
-        <v>55</v>
+      <c r="D102" s="18" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="103" spans="1:4">
-      <c r="A103" s="9" t="s">
-        <v>141</v>
+      <c r="A103" s="28" t="s">
+        <v>36</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>279</v>
+        <v>201</v>
       </c>
       <c r="C103" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4">
-      <c r="A104" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="B104" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="C104" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D104" s="18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4">
-      <c r="A105" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="B105" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="C105" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D105" s="9" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D105">
+  <autoFilter ref="A1:D103">
     <sortState ref="A2:E102">
       <sortCondition ref="D2:D102"/>
     </sortState>

</xml_diff>

<commit_message>
solved hang issue during ping sync
</commit_message>
<xml_diff>
--- a/Echo/Router ip list with 37 SMS numbers.xlsx
+++ b/Echo/Router ip list with 37 SMS numbers.xlsx
@@ -17,14 +17,14 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$105</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="351">
   <si>
     <t>Moghbazar</t>
   </si>
@@ -1071,6 +1071,12 @@
   </si>
   <si>
     <t>192.168.0.207</t>
+  </si>
+  <si>
+    <t>192.168.0.208</t>
+  </si>
+  <si>
+    <t>192.168.0.209</t>
   </si>
 </sst>
 </file>
@@ -1645,11 +1651,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K103"/>
+  <dimension ref="A1:K105"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1680,7 +1686,7 @@
     </row>
     <row r="2" spans="1:11" s="26" customFormat="1">
       <c r="A2" s="12" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>346</v>
@@ -1694,770 +1700,764 @@
     </row>
     <row r="3" spans="1:11" s="26" customFormat="1">
       <c r="A3" s="12" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>341</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>289</v>
+        <v>347</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="26" customFormat="1">
       <c r="A4" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="26" customFormat="1">
+      <c r="A5" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="26" customFormat="1">
+      <c r="A6" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B6" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="C6" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>343</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>259</v>
+        <v>107</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>236</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="K7" s="2"/>
+      <c r="D7" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="12" t="s">
-        <v>122</v>
+        <v>184</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>244</v>
+        <v>274</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="K8" s="1"/>
+        <v>180</v>
+      </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="12" t="s">
-        <v>296</v>
+        <v>165</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>297</v>
+        <v>259</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="K9" s="1"/>
+        <v>147</v>
+      </c>
+      <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="12" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>134</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>251</v>
+        <v>296</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>297</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D11" s="33" t="s">
-        <v>133</v>
-      </c>
+      <c r="D11" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="B12" s="31" t="s">
-        <v>248</v>
+        <v>140</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>252</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D12" s="33" t="s">
-        <v>120</v>
+      <c r="D12" s="11" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="12" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="12" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>119</v>
+      <c r="D14" s="33" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="12" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>270</v>
+        <v>125</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>247</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>158</v>
+      <c r="D16" s="12" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>269</v>
+        <v>130</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>249</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>157</v>
+      <c r="D17" s="33" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="B18" s="31" t="s">
-        <v>268</v>
+        <v>176</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>270</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D18" s="33" t="s">
-        <v>156</v>
+      <c r="D18" s="11" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>235</v>
+        <v>175</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>269</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>94</v>
+      <c r="D19" s="11" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>242</v>
+      <c r="A20" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>268</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D20" s="20" t="s">
-        <v>100</v>
+      <c r="D20" s="33" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="12" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>231</v>
+      <c r="A22" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>242</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D22" s="10" t="s">
-        <v>292</v>
+      <c r="D22" s="20" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="12" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="B24" s="31" t="s">
-        <v>233</v>
+        <v>102</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>231</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D24" s="33" t="s">
-        <v>92</v>
+      <c r="D24" s="10" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>241</v>
+      <c r="A25" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>230</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D25" s="20" t="s">
-        <v>99</v>
+      <c r="D25" s="12" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>234</v>
+        <v>104</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>233</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D26" s="12" t="s">
-        <v>93</v>
+      <c r="D26" s="33" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>239</v>
+      <c r="A27" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>241</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>97</v>
+      <c r="D27" s="20" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>288</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B31" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D29" s="20" t="s">
+      <c r="C31" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D31" s="20" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="15" t="s">
+    <row r="32" spans="1:4">
+      <c r="A32" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B32" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="C30" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D30" s="20" t="s">
+      <c r="C32" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D32" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="20" t="s">
+    <row r="33" spans="1:4">
+      <c r="A33" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B33" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="C31" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D31" s="10" t="s">
+      <c r="C33" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>255</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B36" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="C34" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D34" s="12" t="s">
+      <c r="C36" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D36" s="12" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C38" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D38" s="10" t="s">
+      <c r="C40" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D40" s="10" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D39" s="20" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>265</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="12" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>260</v>
+        <v>171</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>265</v>
       </c>
       <c r="C42" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D42" s="12" t="s">
-        <v>148</v>
+      <c r="D42" s="20" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>253</v>
+        <v>167</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>261</v>
       </c>
       <c r="C43" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D43" s="13" t="s">
-        <v>142</v>
+      <c r="D43" s="20" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>254</v>
+        <v>166</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>260</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D44" s="13" t="s">
-        <v>185</v>
+      <c r="D44" s="12" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B47" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="C45" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D45" s="13" t="s">
+      <c r="C47" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D47" s="13" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="B47" s="30" t="s">
-        <v>224</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D47" s="28" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="9" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>263</v>
+      <c r="A49" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B49" s="30" t="s">
+        <v>224</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D49" s="9" t="s">
-        <v>151</v>
+      <c r="D49" s="28" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>267</v>
+        <v>162</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>256</v>
       </c>
       <c r="C50" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D50" s="9" t="s">
-        <v>155</v>
+      <c r="D50" s="13" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>258</v>
+        <v>169</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>263</v>
       </c>
       <c r="C51" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D51" s="13" t="s">
-        <v>146</v>
+      <c r="D51" s="9" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>264</v>
+        <v>173</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>267</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D52" s="13" t="s">
-        <v>152</v>
+      <c r="D52" s="9" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D54" s="13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B55" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="C53" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D53" s="13" t="s">
+      <c r="C55" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D55" s="13" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="29" t="s">
+    <row r="56" spans="1:6">
+      <c r="A56" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B56" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="C54" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D54" s="13" t="s">
+      <c r="C56" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D56" s="13" t="s">
         <v>9</v>
-      </c>
-      <c r="F54" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="C55" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>0</v>
@@ -2465,16 +2465,16 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="B57" s="30" t="s">
-        <v>209</v>
+        <v>14</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>191</v>
       </c>
       <c r="C57" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D57" s="28" t="s">
-        <v>51</v>
+      <c r="D57" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>0</v>
@@ -2482,16 +2482,16 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B58" s="30" t="s">
-        <v>197</v>
+        <v>18</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>193</v>
       </c>
       <c r="C58" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>0</v>
@@ -2499,16 +2499,16 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>188</v>
+        <v>52</v>
+      </c>
+      <c r="B59" s="30" t="s">
+        <v>209</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D59" s="12" t="s">
-        <v>7</v>
+      <c r="D59" s="28" t="s">
+        <v>51</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>0</v>
@@ -2516,16 +2516,16 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>204</v>
+        <v>25</v>
+      </c>
+      <c r="B60" s="30" t="s">
+        <v>197</v>
       </c>
       <c r="C60" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D60" s="10" t="s">
-        <v>40</v>
+      <c r="D60" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="F60" s="7" t="s">
         <v>0</v>
@@ -2533,16 +2533,16 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="B61" s="30" t="s">
-        <v>186</v>
+        <v>8</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>188</v>
       </c>
       <c r="C61" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D61" s="28" t="s">
-        <v>285</v>
+      <c r="D61" s="12" t="s">
+        <v>7</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>0</v>
@@ -2550,16 +2550,16 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="B62" s="30" t="s">
-        <v>187</v>
+        <v>39</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>204</v>
       </c>
       <c r="C62" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D62" s="28" t="s">
-        <v>4</v>
+      <c r="D62" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="F62" s="7" t="s">
         <v>0</v>
@@ -2567,16 +2567,16 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="28" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="B63" s="30" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="C63" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D63" s="28" t="s">
-        <v>27</v>
+        <v>285</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>0</v>
@@ -2584,31 +2584,33 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="28" t="s">
-        <v>298</v>
+        <v>5</v>
       </c>
       <c r="B64" s="30" t="s">
-        <v>299</v>
+        <v>187</v>
       </c>
       <c r="C64" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D64" s="28" t="s">
-        <v>300</v>
-      </c>
-      <c r="F64" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>192</v>
+        <v>28</v>
+      </c>
+      <c r="B65" s="30" t="s">
+        <v>198</v>
       </c>
       <c r="C65" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D65" s="9" t="s">
-        <v>15</v>
+      <c r="D65" s="28" t="s">
+        <v>27</v>
       </c>
       <c r="F65" s="7" t="s">
         <v>0</v>
@@ -2616,541 +2618,573 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>199</v>
+        <v>298</v>
+      </c>
+      <c r="B66" s="30" t="s">
+        <v>299</v>
       </c>
       <c r="C66" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D66" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F66" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="D66" s="28" t="s">
+        <v>300</v>
+      </c>
+      <c r="F66" s="7"/>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="B67" s="30" t="s">
-        <v>215</v>
+        <v>16</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>192</v>
       </c>
       <c r="C67" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D67" s="28" t="s">
-        <v>62</v>
+      <c r="D67" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="B68" s="30" t="s">
-        <v>205</v>
+        <v>32</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="C68" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D68" s="28" t="s">
-        <v>42</v>
+      <c r="D68" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="28" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B69" s="30" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="C69" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D69" s="28" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B70" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D70" s="28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B71" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D71" s="28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B70" s="30" t="s">
+      <c r="B72" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="C70" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D70" s="28" t="s">
+      <c r="C72" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D72" s="28" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
-      <c r="A71" s="9" t="s">
+    <row r="73" spans="1:6">
+      <c r="A73" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="B73" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="C71" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D71" s="9" t="s">
+      <c r="C73" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D73" s="9" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
-      <c r="A72" s="13" t="s">
+    <row r="74" spans="1:6">
+      <c r="A74" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="B72" s="8" t="s">
+      <c r="B74" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="C72" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D72" s="13" t="s">
+      <c r="C74" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D74" s="13" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
-      <c r="A73" s="13" t="s">
+    <row r="75" spans="1:6">
+      <c r="A75" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="B73" s="8" t="s">
+      <c r="B75" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="C73" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D73" s="13" t="s">
+      <c r="C75" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D75" s="13" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
-      <c r="A74" s="9" t="s">
+    <row r="76" spans="1:6">
+      <c r="A76" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="B74" s="7" t="s">
+      <c r="B76" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="C74" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D74" s="9" t="s">
+      <c r="C76" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D76" s="9" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
-      <c r="A75" s="28" t="s">
+    <row r="77" spans="1:6">
+      <c r="A77" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="B75" s="30" t="s">
+      <c r="B77" s="30" t="s">
         <v>222</v>
       </c>
-      <c r="C75" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D75" s="28" t="s">
+      <c r="C77" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D77" s="28" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
-      <c r="A76" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="B76" s="30" t="s">
-        <v>221</v>
-      </c>
-      <c r="C76" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D76" s="28" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B77" s="32" t="s">
-        <v>220</v>
-      </c>
-      <c r="C77" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D77" s="35" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="28" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B78" s="30" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C78" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D78" s="28" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:6">
-      <c r="A79" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="B79" s="30" t="s">
-        <v>225</v>
+      <c r="A79" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B79" s="32" t="s">
+        <v>220</v>
       </c>
       <c r="C79" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D79" s="28" t="s">
-        <v>83</v>
+      <c r="D79" s="35" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="28" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B80" s="30" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C80" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>227</v>
+        <v>81</v>
+      </c>
+      <c r="B81" s="30" t="s">
+        <v>225</v>
       </c>
       <c r="C81" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D81" s="9" t="s">
-        <v>85</v>
+      <c r="D81" s="28" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>229</v>
+        <v>77</v>
+      </c>
+      <c r="B82" s="30" t="s">
+        <v>223</v>
       </c>
       <c r="C82" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D82" s="9" t="s">
-        <v>87</v>
+      <c r="D82" s="28" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="B83" s="30" t="s">
-        <v>219</v>
+        <v>88</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>227</v>
       </c>
       <c r="C83" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D83" s="28" t="s">
-        <v>72</v>
+      <c r="D83" s="9" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="28" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C84" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="28" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B85" s="30" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C85" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D85" s="37" t="s">
-        <v>64</v>
+      <c r="D85" s="28" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="B86" s="30" t="s">
-        <v>217</v>
+        <v>89</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>228</v>
       </c>
       <c r="C86" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D86" s="28" t="s">
-        <v>70</v>
+      <c r="D86" s="9" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B87" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="C87" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D87" s="37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B88" s="30" t="s">
+        <v>217</v>
+      </c>
+      <c r="C88" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D88" s="28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="28" t="s">
         <v>301</v>
       </c>
-      <c r="B87" s="30" t="s">
+      <c r="B89" s="30" t="s">
         <v>302</v>
       </c>
-      <c r="C87" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D87" s="37" t="s">
+      <c r="C89" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D89" s="37" t="s">
         <v>303</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
-      <c r="A88" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="B88" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="C88" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D88" s="9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="B89" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="C89" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D89" s="9" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="9" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>278</v>
+        <v>246</v>
       </c>
       <c r="C90" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D90" s="19" t="s">
-        <v>283</v>
+      <c r="D90" s="9" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="9" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
       <c r="C91" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="C92" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D92" s="19" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C93" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D93" s="9" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="B92" s="7" t="s">
+      <c r="B94" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="C92" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D92" s="9" t="s">
+      <c r="C94" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D94" s="9" t="s">
         <v>282</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
-      <c r="A93" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B93" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="C93" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D93" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4">
-      <c r="A94" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B94" s="30" t="s">
-        <v>202</v>
-      </c>
-      <c r="C94" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D94" s="28" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="B95" s="30" t="s">
-        <v>208</v>
+        <v>34</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>203</v>
       </c>
       <c r="C95" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D95" s="28" t="s">
-        <v>48</v>
+      <c r="D95" s="9" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="28" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="B96" s="30" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="C96" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D96" s="36" t="s">
-        <v>58</v>
+      <c r="D96" s="28" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="28" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B97" s="30" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C97" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D97" s="28" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="28" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B98" s="30" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C98" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D98" s="34" t="s">
-        <v>53</v>
+      <c r="D98" s="36" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="28" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B99" s="30" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C99" s="10" t="s">
         <v>341</v>
       </c>
       <c r="D99" s="28" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B100" s="30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C100" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D100" s="10" t="s">
-        <v>55</v>
+      <c r="D100" s="34" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="B101" s="7" t="s">
-        <v>279</v>
+      <c r="A101" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B101" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C101" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="D101" s="9" t="s">
-        <v>284</v>
+      <c r="D101" s="28" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B102" s="30" t="s">
+        <v>212</v>
+      </c>
+      <c r="C102" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D102" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="C103" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D103" s="9" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B102" s="7" t="s">
+      <c r="B104" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="C102" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D102" s="18" t="s">
+      <c r="C104" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D104" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
-      <c r="A103" s="28" t="s">
+    <row r="105" spans="1:4">
+      <c r="A105" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B103" s="7" t="s">
+      <c r="B105" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="C103" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D103" s="9" t="s">
+      <c r="C105" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D105" s="9" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D103">
+  <autoFilter ref="A1:D105">
     <sortState ref="A2:E102">
       <sortCondition ref="D2:D102"/>
     </sortState>

</xml_diff>

<commit_message>
SMS halt added for no phone number
</commit_message>
<xml_diff>
--- a/Echo/Router ip list with 37 SMS numbers.xlsx
+++ b/Echo/Router ip list with 37 SMS numbers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
@@ -1348,10 +1348,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1660,13 +1660,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1714,12 +1715,6 @@
       <c r="D3" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="26">
-        <v>1917300427</v>
-      </c>
-      <c r="F3" s="26">
-        <v>1571797880</v>
-      </c>
     </row>
     <row r="4" spans="1:11" s="26" customFormat="1">
       <c r="A4" s="12" t="s">
@@ -1876,8 +1871,12 @@
       <c r="D11" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
+      <c r="E11" s="26">
+        <v>1917300427</v>
+      </c>
+      <c r="F11" s="26">
+        <v>1571797880</v>
+      </c>
       <c r="G11" s="26"/>
     </row>
   </sheetData>
@@ -1889,9 +1888,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1921,12 +1920,12 @@
       <c r="D1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="38" t="s">
         <v>347</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:11" s="26" customFormat="1">
       <c r="A2" s="12" t="s">

</xml_diff>

<commit_message>
Added phone list on UI
</commit_message>
<xml_diff>
--- a/Echo/Router ip list with 37 SMS numbers.xlsx
+++ b/Echo/Router ip list with 37 SMS numbers.xlsx
@@ -1247,7 +1247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1354,6 +1354,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1658,10 +1659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1669,9 +1670,11 @@
     <col min="2" max="2" width="16.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="21" customFormat="1">
+    <row r="1" spans="1:15" s="21" customFormat="1">
       <c r="A1" s="22" t="s">
         <v>292</v>
       </c>
@@ -1685,7 +1688,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="26" customFormat="1">
+    <row r="2" spans="1:15" s="26" customFormat="1">
       <c r="A2" s="12" t="s">
         <v>344</v>
       </c>
@@ -1701,8 +1704,11 @@
       <c r="E2" s="26">
         <v>1917300427</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" s="26" customFormat="1">
+      <c r="F2" s="26">
+        <v>1571797880</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="26" customFormat="1">
       <c r="A3" s="12" t="s">
         <v>341</v>
       </c>
@@ -1715,8 +1721,11 @@
       <c r="D3" s="6" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" s="26" customFormat="1">
+      <c r="E3" s="26">
+        <v>1917300427</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="26" customFormat="1">
       <c r="A4" s="12" t="s">
         <v>339</v>
       </c>
@@ -1735,8 +1744,35 @@
       <c r="F4" s="26">
         <v>1571797880</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="G4" s="26">
+        <v>545454545</v>
+      </c>
+      <c r="H4" s="40">
+        <v>656565</v>
+      </c>
+      <c r="I4" s="40">
+        <v>6565656</v>
+      </c>
+      <c r="J4" s="40">
+        <v>5656565</v>
+      </c>
+      <c r="K4" s="40">
+        <v>5656565</v>
+      </c>
+      <c r="L4" s="40">
+        <v>56565656</v>
+      </c>
+      <c r="M4" s="40">
+        <v>565656565</v>
+      </c>
+      <c r="N4" s="40">
+        <v>4654445</v>
+      </c>
+      <c r="O4" s="40">
+        <v>6565655</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="12" t="s">
         <v>106</v>
       </c>
@@ -1760,7 +1796,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:15">
       <c r="A6" s="12" t="s">
         <v>181</v>
       </c>
@@ -1779,7 +1815,7 @@
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:15">
       <c r="A7" s="12" t="s">
         <v>162</v>
       </c>
@@ -1799,7 +1835,7 @@
       <c r="G7" s="26"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:15">
       <c r="A8" s="12" t="s">
         <v>121</v>
       </c>
@@ -1819,7 +1855,7 @@
       <c r="G8" s="26"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:15">
       <c r="A9" s="12" t="s">
         <v>293</v>
       </c>
@@ -1839,7 +1875,7 @@
       <c r="G9" s="26"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:15">
       <c r="A10" s="12" t="s">
         <v>345</v>
       </c>
@@ -1858,7 +1894,7 @@
       <c r="F10" s="26"/>
       <c r="G10" s="26"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:15">
       <c r="A11" s="12" t="s">
         <v>346</v>
       </c>
@@ -1872,11 +1908,9 @@
         <v>132</v>
       </c>
       <c r="E11" s="26">
-        <v>1917300427</v>
-      </c>
-      <c r="F11" s="26">
         <v>1571797880</v>
       </c>
+      <c r="F11" s="26"/>
       <c r="G11" s="26"/>
     </row>
   </sheetData>
@@ -1890,7 +1924,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>